<commit_message>
Agregado modificar y buscar
Agregada la implementación de los métodos
-Modificar libro
-Buscar libro
</commit_message>
<xml_diff>
--- a/Documentacion/Requerimientos.xlsx
+++ b/Documentacion/Requerimientos.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
     <sheet name="Caso de uso H1" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Caso de uso H2" sheetId="3" r:id="rId3"/>
+    <sheet name="Caso de uso H3" sheetId="5" r:id="rId4"/>
+    <sheet name="Caso de uso H5" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="162">
   <si>
     <t>Titulo</t>
   </si>
@@ -126,9 +128,6 @@
     <t>22.- El sistema guarda la sinopsis del libro</t>
   </si>
   <si>
-    <t>23.- El libro es agregado a la lista del inventario</t>
-  </si>
-  <si>
     <t>3.1 El usuario no introduce el título del libro o introduce uno no válido</t>
   </si>
   <si>
@@ -172,13 +171,346 @@
   </si>
   <si>
     <t>19.2.- Se almacena 0 como número de páginas</t>
+  </si>
+  <si>
+    <t>Como usuario quisiera poder buscar libros por autor o titulo</t>
+  </si>
+  <si>
+    <t>1.- El usuario selecciona la opción correspondiente a eliminar libro</t>
+  </si>
+  <si>
+    <t>2.- El sistema muestra un listado indexado de los libros almacenados</t>
+  </si>
+  <si>
+    <t>24.- El libro es agregado a la lista del inventario</t>
+  </si>
+  <si>
+    <t>23.- El sistema pide confirmación de la operación</t>
+  </si>
+  <si>
+    <t>3.- El sistema pide El numero de libro a eliminar</t>
+  </si>
+  <si>
+    <t>4.- El usuario selecciona el número del libro que desea eliminar</t>
+  </si>
+  <si>
+    <t>5.- El sistema pide que se confirme la operación</t>
+  </si>
+  <si>
+    <t>6.- El usuario confirma la operacion</t>
+  </si>
+  <si>
+    <t>7.- El sistema elimina el libro del inventario</t>
+  </si>
+  <si>
+    <t>6.1.- El usuario niega la operación</t>
+  </si>
+  <si>
+    <t>4.1.- El usuario selecciona una opción no válida</t>
+  </si>
+  <si>
+    <t>4.2 regresa al paso 3</t>
+  </si>
+  <si>
+    <t>Camino Alterno</t>
+  </si>
+  <si>
+    <t>1.- El usuario selecciona la opción correspondiente a buscar libro</t>
+  </si>
+  <si>
+    <t>3.- El usuario introduce el título</t>
+  </si>
+  <si>
+    <t>2.- El sistema pide el título</t>
+  </si>
+  <si>
+    <t>4.- El sistema pide el autor</t>
+  </si>
+  <si>
+    <t>5.- El usuario introduce al autor</t>
+  </si>
+  <si>
+    <t>5.1.- El usuario no introduce un autor</t>
+  </si>
+  <si>
+    <t>3.1.- El usuario no introduce un título</t>
+  </si>
+  <si>
+    <t>3.2.- El título es ignorado en la búsqueda</t>
+  </si>
+  <si>
+    <t>5.2.- El autor es ignorado en la búqueda</t>
+  </si>
+  <si>
+    <t>Nota: Si ningún parámetro de búsqueda es introducido, la búsqueda es cancelada.</t>
+  </si>
+  <si>
+    <t>9.1.1.- El usuario introduce un carácter incorrecto</t>
+  </si>
+  <si>
+    <t>9.1.2.- Regresa paso 8</t>
+  </si>
+  <si>
+    <t>9.2 La editorial es ignorada en la búsqueda</t>
+  </si>
+  <si>
+    <t>12.2.- El formato es ignorado en la búsqueda</t>
+  </si>
+  <si>
+    <t>12.1.1.- El usuario introduce un carácter incorrecto</t>
+  </si>
+  <si>
+    <t>12.1.2.- Regresa paso 11</t>
+  </si>
+  <si>
+    <t>14.1.- El usuario no introduce la edición</t>
+  </si>
+  <si>
+    <t>14.2.- La edición es ignorada para la búsqueda</t>
+  </si>
+  <si>
+    <t>14.1.1.- El usuario introduce un cáracter no numerico</t>
+  </si>
+  <si>
+    <t>14.1.2.- Regresa al paso 13</t>
+  </si>
+  <si>
+    <t>6.- El sistema pide la editorial</t>
+  </si>
+  <si>
+    <t>7.- El sistema despliega una lista con índice de las editoriales</t>
+  </si>
+  <si>
+    <t>8.- El usuario introduce el número de una editorial</t>
+  </si>
+  <si>
+    <t>9.- El sistema pide el formato</t>
+  </si>
+  <si>
+    <t>10.- El sistema despliega una lista con índice de los formatos</t>
+  </si>
+  <si>
+    <t>11. El usuario introduce el número de un formato</t>
+  </si>
+  <si>
+    <t>12.- El sistema pide la  edición del libro</t>
+  </si>
+  <si>
+    <t>13.- El usuario introduce la edicion del libro</t>
+  </si>
+  <si>
+    <t>14.- El sistema regresa un lista con los libros que coincidieron</t>
+  </si>
+  <si>
+    <t>9.1.- El usuario no introduce nada</t>
+  </si>
+  <si>
+    <t>12.1.- El usuario no introduce nada</t>
+  </si>
+  <si>
+    <t>Como usuario quisiera poder buscar libros</t>
+  </si>
+  <si>
+    <t>Num</t>
+  </si>
+  <si>
+    <t>1.- El usuario selecciona la opción del menú correspondiente a modificar</t>
+  </si>
+  <si>
+    <t>Modificaciones:</t>
+  </si>
+  <si>
+    <t>El sistema puede pedir el num del libro</t>
+  </si>
+  <si>
+    <t>2.- El sistema muestra un listado de los libros disponibles con un índice</t>
+  </si>
+  <si>
+    <t>3.- El usuario introduce el número del libro que desea modificar</t>
+  </si>
+  <si>
+    <t>4.- El sistema muestra el título original del libro</t>
+  </si>
+  <si>
+    <t>5.- El sistema pide el nuevo título del libro</t>
+  </si>
+  <si>
+    <t>6.- El usuario introduce el nuevo título</t>
+  </si>
+  <si>
+    <t>7.- El sistema muestra el autor original del libro</t>
+  </si>
+  <si>
+    <t>8.- El sistema pide el nuevo autor del libro</t>
+  </si>
+  <si>
+    <t>9.- El usuario introduce el nuevo autor del libro</t>
+  </si>
+  <si>
+    <t>10.- El sistema muestra la editorial original del libro</t>
+  </si>
+  <si>
+    <t>11.- El sistema pide la nueva editorial</t>
+  </si>
+  <si>
+    <t>12.- El sistema muestra una lista indexada de las editoriales</t>
+  </si>
+  <si>
+    <t>13.- El usuario introduce el número de la nueva editorial</t>
+  </si>
+  <si>
+    <t>13.- El sistema muestra el formato original del libro</t>
+  </si>
+  <si>
+    <t>14.- El sistema pide el nuevo formato</t>
+  </si>
+  <si>
+    <t>15.- El sistema muestra una lista indexada de los formatos</t>
+  </si>
+  <si>
+    <t>16.- El usuario introduce el número del nuevo formato</t>
+  </si>
+  <si>
+    <t>17.- El sistema muestra la edicion original del libro</t>
+  </si>
+  <si>
+    <t>19.- El usuario introduce la nueva edición del libro</t>
+  </si>
+  <si>
+    <t>18.- El sistema pide la nueva edición del libro</t>
+  </si>
+  <si>
+    <t>20.- El sistema muestra el número ISBN original del libro</t>
+  </si>
+  <si>
+    <t>21.- El sistema pide el nuevo número ISBN del libro</t>
+  </si>
+  <si>
+    <t>22.- El usuario introduce el nuevo número ISBN del libro</t>
+  </si>
+  <si>
+    <t>23.- El sistema muestra el número de páginas original del libro</t>
+  </si>
+  <si>
+    <t>24.- El sistema pide el nuevo número de páginas del libro</t>
+  </si>
+  <si>
+    <t>25.- El usuario introduce el nuevo número de páginas del libro</t>
+  </si>
+  <si>
+    <t>26.- El sistema muestra la sinopsis original del libro</t>
+  </si>
+  <si>
+    <t>27.- El sistema pide la nueva sinopsis del libro</t>
+  </si>
+  <si>
+    <t>28.- El sistema muestra un resumen de los datos</t>
+  </si>
+  <si>
+    <t>29.- El usuario confirma los datos</t>
+  </si>
+  <si>
+    <t>30.- El sistema remplaza los datos del libro modificado</t>
+  </si>
+  <si>
+    <t>3.1.- El usuario introduce una carácter no válido</t>
+  </si>
+  <si>
+    <t>3.2.- Regresa a paso 2</t>
+  </si>
+  <si>
+    <t>6.1.- El usuario no introduce el título del lbro</t>
+  </si>
+  <si>
+    <t>6.2 El sistema ignora la modificación</t>
+  </si>
+  <si>
+    <t>8.1.- El usuario no introduce el nuevo autor</t>
+  </si>
+  <si>
+    <t>8.2.- El sistema ignora la modificacion</t>
+  </si>
+  <si>
+    <t>13.2.- El sistema ignora la modificación</t>
+  </si>
+  <si>
+    <t>13.1.- El usuario no introduce nada</t>
+  </si>
+  <si>
+    <t>13.1.1.- El usuario introduce un carácter no válido</t>
+  </si>
+  <si>
+    <t>16.1.- El usuario no introduce nada</t>
+  </si>
+  <si>
+    <t>16.1.1.- El usuario introduce un carácter no válido</t>
+  </si>
+  <si>
+    <t>19.1.- El usuario no introduce nada</t>
+  </si>
+  <si>
+    <t>13.1.2.- Regresa al paso 12</t>
+  </si>
+  <si>
+    <t>16.1.2.- Regresa al paso 15</t>
+  </si>
+  <si>
+    <t>19.2.- El sistema ignora la modificación</t>
+  </si>
+  <si>
+    <t>19.1.1.- El usuario introduce un carácter no válido</t>
+  </si>
+  <si>
+    <t>22.1.- El usuario no introduce nada</t>
+  </si>
+  <si>
+    <t>22.2.- El sistema ignora la modificación</t>
+  </si>
+  <si>
+    <t>22.1.1.- El usuario introduce un ISBN malo</t>
+  </si>
+  <si>
+    <t>22.1.2.- Regresa al paso 21</t>
+  </si>
+  <si>
+    <t>25.1.- El usuario no introduce nada</t>
+  </si>
+  <si>
+    <t>25.1.- El sistema ignora la modificación</t>
+  </si>
+  <si>
+    <t>25.1.1.- El usuario introduce un número no válido</t>
+  </si>
+  <si>
+    <t>25.1.2.- Regresa al paso 22</t>
+  </si>
+  <si>
+    <t>27.1.- El usuario no introduce nada</t>
+  </si>
+  <si>
+    <t>27.1.- El sistema ignora la modificación</t>
+  </si>
+  <si>
+    <t>29.1.- El usuario no confiema los datos</t>
+  </si>
+  <si>
+    <t>29.2.- El sistema ignora las modificaciones</t>
+  </si>
+  <si>
+    <t>29.1.1.- El usuario introduce un carácer no válido</t>
+  </si>
+  <si>
+    <t>Hacer un seleccionador de libros</t>
+  </si>
+  <si>
+    <t>Hacer un seleccionador de Formatos y Editoriales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,8 +526,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +566,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -233,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -251,6 +633,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,72 +948,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C4" s="7"/>
+      <c r="D4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="8"/>
+      <c r="D5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="7"/>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,130 +1065,127 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>13</v>
+      <c r="E4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="G18" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" t="s">
-        <v>47</v>
-      </c>
-      <c r="H19" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G20" t="s">
+        <v>46</v>
       </c>
       <c r="H20" t="s">
         <v>45</v>
@@ -768,49 +1193,62 @@
     </row>
     <row r="21" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="H21" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H23" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="G25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -821,12 +1259,531 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" t="s">
+        <v>148</v>
+      </c>
+      <c r="D26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" t="s">
+        <v>152</v>
+      </c>
+      <c r="D29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>